<commit_message>
add skeleton for jms, shortest path and positioning
</commit_message>
<xml_diff>
--- a/IHNdoc/spec/demo_requirement.xlsx
+++ b/IHNdoc/spec/demo_requirement.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="要点" sheetId="1" r:id="rId1"/>
     <sheet name="需求" sheetId="2" r:id="rId2"/>
+    <sheet name="addition" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>架构</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,10 +182,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>baidu map API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>点击某个物业的百度地图图标进入到该物业的管理界面</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -231,24 +228,126 @@
   <si>
     <t>物业操作员可修改物业map，包括：标注车位，各个可管对象</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下拉菜单, filter</t>
+  </si>
+  <si>
+    <t>页面风格,layout (左边列表，右边baidu map), 点击某个地方弹出操作菜单</t>
+  </si>
+  <si>
+    <t>点击某个node,弹出一个窗口: property information, play video…/tab page</t>
+  </si>
+  <si>
+    <t>个人设置: write to local storage, sdcard or /data/data/ihn/setting.properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本地地图管理:   /data/data/ihn/maps/parking1/[resource | json]
+概要信息 </t>
+  </si>
+  <si>
+    <t>bluetooth信号判断当前的位置（车位，层数）</t>
+  </si>
+  <si>
+    <t>baidu map API (同一地图上标注多个车库)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">获取SDCard的状态：Environment.getExtemalStorageState() 
+  EnvironmentMEDIA_MOUNTED手机 装有SDCard，并且可以进行读写 
+获取SDCard的目录：Environment.getExtemalStorageDirectory() </t>
+  </si>
+  <si>
+    <t>&lt;permission name="android.permission.WRITE_EXTERNAL_STORAGE" &gt; 
+        &lt;group gid="sdcard_rw" /&gt; 
+    &lt;/permission&gt;</t>
+  </si>
+  <si>
+    <t>在sdcard中创建/删除文件的权限用android.permission.MOUNT_UNMOUNT_FILESYSTEMS</t>
+  </si>
+  <si>
+    <t>http://wenku.baidu.com/view/f953de8cd0d233d4b14e69ce.html</t>
+  </si>
+  <si>
+    <t>layer1: map</t>
+  </si>
+  <si>
+    <t>layer2: parking place</t>
+  </si>
+  <si>
+    <t>layer3: device</t>
+  </si>
+  <si>
+    <t>计算2个点的最近距离: graph, point, edge, 最短距离算法 (Dijkstra)</t>
+  </si>
+  <si>
+    <t>直线还好，如果是不规则形状，或者曲线，弧线就比较难计算(有限切分为直线)</t>
+  </si>
+  <si>
+    <t>layer4: walking route(point, edge)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">function showInfo(e){
+  alert(e.point.lng + ", " + e.point.lat);
+ }
+ map.addEventListener("click", showInfo);
+ ====
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>var marker = new BMap.Marker(new BMap.Point(116.404, 39.915)); // 创建点
+ marker.addEventListener("click",attribute);
+ map.addOverlay(marker);    //增加点</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ function attribute(){
+  var p = marker.getPosition();  //获取marker的位置
+  alert("marker的位置是" + p.lng + "," + p.lat);    
+ }</t>
+    </r>
+  </si>
+  <si>
+    <t>支持中，英文</t>
+  </si>
+  <si>
+    <t>与物业系统进行数据的实时或批量的sync (batch, jms messaging)</t>
+  </si>
+  <si>
+    <t>simulator to send park space is occupied.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -256,7 +355,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -264,7 +363,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -272,9 +371,25 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -295,12 +410,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -319,17 +437,208 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2819400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>208950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>151861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8439150" y="1990725"/>
+          <a:ext cx="4800000" cy="4314286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>237624</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>75534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11058525" y="6429375"/>
+          <a:ext cx="4009524" cy="5333334"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1038225</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304416</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>85424</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6657975" y="8229600"/>
+          <a:ext cx="3076191" cy="2409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4471639</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5690839" cy="2524125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -403,6 +712,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -437,6 +747,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -612,18 +923,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -677,7 +988,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="25.5">
       <c r="A8" s="2"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -754,18 +1065,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="69.875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="57.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="69.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -882,70 +1193,190 @@
         <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="25.5">
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="B24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="B25" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="25.5">
+      <c r="B26" s="3" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="B26" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="B27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="51">
+      <c r="B39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="51">
+      <c r="B40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="C41" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="15">
+      <c r="B45" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B45" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C16:C23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="87.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="16" spans="3:3">
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" ht="195">
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>